<commit_message>
Pajas, ahora si terminé
</commit_message>
<xml_diff>
--- a/Barbie_Financiera_FASE_2/Reporte de Defectos RP 2.xlsx
+++ b/Barbie_Financiera_FASE_2/Reporte de Defectos RP 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esenedusv-my.sharepoint.com/personal/20235894_esen_edu_sv/Documents/PDS/Proyecto/Proyecto-PDS-BarbieFinanciera/Barbie_Financiera_FASE_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{AF4586E8-5897-42D6-B25A-A5DE437132F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{385CB410-DEC1-4995-B623-2EEE1E9F3211}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{AF4586E8-5897-42D6-B25A-A5DE437132F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02A26CB6-0D2E-4A1B-ABB7-36DBAA7906EA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defectos" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>ID del Defecto</t>
   </si>
@@ -160,12 +160,55 @@
   <si>
     <t>BF-0042-DE007</t>
   </si>
+  <si>
+    <t>DE-01-CDP-02-BF-0043</t>
+  </si>
+  <si>
+    <t>DE-02-CDP-02-BF-0043</t>
+  </si>
+  <si>
+    <t>DE-03-CDP-02-BF-0043</t>
+  </si>
+  <si>
+    <t>DE-04-CDP-02-BF-0043</t>
+  </si>
+  <si>
+    <t>Al momento de seleccionar el nombre de la categoria a la cual se desea crear, no aparece en la seccion, y aunque si se crea la categoria con el monto asignado.</t>
+  </si>
+  <si>
+    <t>En el momento que uno entra al apartado "Detalles de Categorías" se espera que se posea el monto del presupuesto general resultante.</t>
+  </si>
+  <si>
+    <t>Al momento que se procede a observar los detalles de las categorias, este no posee los detalles de los movimientos para, tampoco refleja el saldo resultado de la categoria, puesto que no se han hecho cambios o movimientos.</t>
+  </si>
+  <si>
+    <t>Al momento de intentar realizar cambios o movimientos para cambiar los saldos de las categorias y consigo mismo tambien el monto resultante general al ver se los cambios, no se genera ya que no posee funcionalidades para crear estas salidas de flujo.</t>
+  </si>
+  <si>
+    <t>Módulo de Detalles de Categorías</t>
+  </si>
+  <si>
+    <t>ID: BF-0043: Como usuario, quiero ver un resumen de mi presupuesto, incluyendo
+cuánto he gastado y cuánto me queda disponible por categoría para llevar un control claro de mis finanzas</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Ricardo Cubias</t>
+  </si>
+  <si>
+    <t>El sistema no posee la funcionalidad de movientos para poder observar el saldo restante de la categoria y del presupuesto general.</t>
+  </si>
+  <si>
+    <t>El sistema no posee la funcionalidad de movientos para poder observar los cambios de manera automatica del saldo restante de la categoria y del presupuesto general.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -205,8 +248,14 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,118 +298,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -384,7 +334,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -394,65 +344,149 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCD2D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCD2D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1580,13 +1614,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="51" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
@@ -1595,310 +1629,386 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="152.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="19">
         <v>45546</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="161.25" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="19">
         <v>45546</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="21">
         <v>45576</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="152.1" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="19">
         <v>45546</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="140.1" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="19">
         <v>45546</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="89.25">
+      <c r="A6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="19">
+        <v>45606</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="97.5" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="19">
+        <v>45606</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="138.75" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="19">
+        <v>45606</v>
+      </c>
+      <c r="J8" s="20"/>
+      <c r="K8" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="174" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="19">
+        <v>45606</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1914,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1938,58 +2048,55 @@
     </row>
     <row r="5" spans="1:3" ht="15">
       <c r="A5" s="2"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9">
-        <f>2+2</f>
-        <v>4</v>
+      <c r="C5" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15">
       <c r="A6" s="2"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="7">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12">
-        <f>2+2</f>
-        <v>4</v>
+      <c r="C7" s="7">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="7">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="5">
         <f>0+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="10">
-        <f>2-1+2</f>
-        <v>3</v>
+      <c r="C12" s="5">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>